<commit_message>
squadlist gets generated, rest is missing
</commit_message>
<xml_diff>
--- a/templates/Wettkampfplan.xlsx
+++ b/templates/Wettkampfplan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Entwicklung\saarTURNier-utils\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miba01\Documents\DFKI\Projects\saarTURNier\saarTURNier-utils\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Durchgang</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Riegeneinteilung</t>
+  </si>
+  <si>
+    <t>Verein</t>
   </si>
 </sst>
 </file>
@@ -348,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -375,19 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -398,6 +392,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,13 +425,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -734,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,216 +761,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="21" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="21" t="s">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="21" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="21" t="s">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="21" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="21" t="s">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="21" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="21" t="s">
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="22" t="s">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C19" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D20" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="D23" s="29" t="s">
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="D21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="29" t="s">
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D23" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="D26" s="29" t="s">
+    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="D24" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="29" t="s">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="25" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="39"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A25:A27"/>
+  <mergeCells count="24">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A23:A25"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
continued with competition planning list
</commit_message>
<xml_diff>
--- a/templates/Wettkampfplan.xlsx
+++ b/templates/Wettkampfplan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miba01\Documents\DFKI\Projects\saarTURNier\saarTURNier-utils\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Entwicklung\saarTURNier-utils\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Durchgang</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Verein</t>
+  </si>
+  <si>
+    <t>KaRi 3</t>
+  </si>
+  <si>
+    <t>KaRi 4</t>
   </si>
 </sst>
 </file>
@@ -174,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -347,6 +353,131 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -354,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -385,25 +516,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,13 +556,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -749,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,14 +897,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="21" t="s">
@@ -776,23 +912,23 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -810,7 +946,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="11"/>
@@ -822,7 +958,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="13"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -832,7 +968,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="16"/>
@@ -844,7 +980,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="17"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -854,7 +990,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="11"/>
@@ -866,7 +1002,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="13"/>
       <c r="C12" s="19"/>
       <c r="D12" s="7"/>
@@ -876,7 +1012,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="11"/>
@@ -888,7 +1024,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="13"/>
       <c r="C14" s="7"/>
       <c r="D14" s="19"/>
@@ -897,164 +1033,184 @@
         <v>10</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+    </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="F20" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="D21" s="25" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="F21" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="25" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="F23" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="D24" s="25" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="F24" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="25" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="45"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="47"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="29"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
+  <mergeCells count="8">
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished referee table generation
</commit_message>
<xml_diff>
--- a/templates/Wettkampfplan.xlsx
+++ b/templates/Wettkampfplan.xlsx
@@ -180,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -478,6 +478,17 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -485,17 +496,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -529,33 +533,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -568,6 +545,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -885,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,309 +911,317 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="40"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="52">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="53">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="53">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="54">
         <v>4</v>
       </c>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="20" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="20" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="20" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="20" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="20" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="20" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="20" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="F20" s="23" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="F20" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="F21" s="23" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="F21" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23" t="s">
+      <c r="A22" s="43"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="F23" s="23" t="s">
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="F23" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="F24" s="23" t="s">
+      <c r="A24" s="43"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="F24" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="23" t="s">
+      <c r="A25" s="43"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="45"/>
+      <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="49"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="49"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="F37" s="21"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="49"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="49"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="29"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Increased number of maximum teams to 15
</commit_message>
<xml_diff>
--- a/templates/Wettkampfplan.xlsx
+++ b/templates/Wettkampfplan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Entwicklung\saarTURNier-utils\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miba01\Documents\SaarTURNier\saarTURNier-utils\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB59242D-5A00-4D7C-B518-34B8F3D32A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,10 +370,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -383,29 +391,7 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -414,7 +400,44 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -422,12 +445,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -435,7 +491,18 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -444,86 +511,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -531,23 +526,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -555,16 +550,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,26 +569,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,14 +606,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -639,7 +633,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -934,14 +928,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="19.7109375" customWidth="1"/>
@@ -949,14 +943,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="17" t="s">
@@ -971,42 +965,42 @@
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="24"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="26"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="28">
+      <c r="B6" s="26">
         <v>1</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="27">
         <v>2</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="27">
         <v>3</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>4</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="7"/>
@@ -1018,7 +1012,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1028,7 +1022,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="12"/>
@@ -1040,7 +1034,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="13"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1050,7 +1044,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="7"/>
@@ -1062,7 +1056,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="9"/>
       <c r="C12" s="15"/>
       <c r="D12" s="3"/>
@@ -1072,7 +1066,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="7"/>
@@ -1084,7 +1078,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="9"/>
       <c r="C14" s="3"/>
       <c r="D14" s="15"/>
@@ -1094,7 +1088,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1105,91 +1099,91 @@
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="24"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1200,107 +1194,109 @@
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="24"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="41"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="34"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="41"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="35"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="41"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="36"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="41"/>
+      <c r="A33" s="51"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="36"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="41"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="36"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="41"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="36"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="41"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="36"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="41"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="36"/>
       <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="41"/>
+      <c r="A38" s="51"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="36"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="41"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="36"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="41"/>
+      <c r="A40" s="51"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="36"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="41"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="41"/>
+      <c r="A41" s="51"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="36"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="41"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="36"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="52"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="36"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="53"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>